<commit_message>
Adds variable line parameter scaling.
With the SBase parameter in the standart_parameter_yml file the line parameter scaling can now be adjusted. Also updates the amount of available line sets.
</commit_message>
<xml_diff>
--- a/data_preparation/standard_line_parameters.xlsx
+++ b/data_preparation/standard_line_parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\V2G-QUESTS\data_preparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5F1948-D4B1-4137-B690-EB440230A3F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367D2938-19E9-4BE8-A7EE-BD0BC6249AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34450" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -410,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.9375" defaultRowHeight="14.35"/>
@@ -446,10 +446,10 @@
         <v>535</v>
       </c>
       <c r="B2" s="3">
-        <v>7.7457152083333328E-2</v>
+        <v>8.4994033412887832E-2</v>
       </c>
       <c r="C2" s="3">
-        <v>0.10199999999999999</v>
+        <v>0.41414671814671816</v>
       </c>
       <c r="D2">
         <f>A2</f>
@@ -465,226 +465,247 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>300</v>
+        <v>419</v>
       </c>
       <c r="B3" s="3">
-        <v>0.108000003</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0.101000004</v>
+        <v>0.13</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.63800000000000001</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D12" si="0">A3</f>
-        <v>300</v>
+        <v>419</v>
       </c>
       <c r="E3" s="2">
         <v>21000</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F12" si="1">(E3*D3*SQRT(3))/1000000</f>
-        <v>10.911920087683926</v>
+        <f>(E3*D3*SQRT(3))/1000000</f>
+        <v>15.240315055798551</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>240</v>
-      </c>
-      <c r="B4" s="4">
-        <v>0.12999999500000001</v>
+        <v>300</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.108000003</v>
       </c>
       <c r="C4" s="4">
-        <v>0.32600000499999998</v>
+        <v>0.101000004</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>240</v>
+        <f t="shared" ref="D4:D13" si="0">A4</f>
+        <v>300</v>
       </c>
       <c r="E4" s="2">
         <v>21000</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" si="1"/>
-        <v>8.7295360701471409</v>
+        <f t="shared" ref="F4:F13" si="1">(E4*D4*SQRT(3))/1000000</f>
+        <v>10.911920087683926</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>185</v>
+        <v>240</v>
       </c>
       <c r="B5" s="4">
-        <v>0.17700000099999999</v>
+        <v>0.12999999500000001</v>
       </c>
       <c r="C5" s="4">
-        <v>0.333999991</v>
+        <v>0.32600000499999998</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>185</v>
+        <v>240</v>
       </c>
       <c r="E5" s="2">
         <v>21000</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="1"/>
-        <v>6.7290173874050883</v>
+        <v>8.7295360701471409</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="B6" s="4">
-        <v>0.209999993</v>
+        <v>0.17700000099999999</v>
       </c>
       <c r="C6" s="4">
-        <v>0.340999991</v>
+        <v>0.333999991</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="E6" s="2">
         <v>21000</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="1"/>
-        <v>5.4559600438419631</v>
+        <v>6.7290173874050883</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="B7" s="4">
-        <v>0.27300000200000002</v>
+        <v>0.209999993</v>
       </c>
       <c r="C7" s="4">
-        <v>0.119999997</v>
+        <v>0.340999991</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="E7" s="2">
         <v>21000</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="1"/>
-        <v>4.3647680350735705</v>
+        <v>5.4559600438419631</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="B8" s="4">
-        <v>0.33000001299999998</v>
+        <v>0.27300000200000002</v>
       </c>
       <c r="C8" s="4">
-        <v>7.8000001999999999E-2</v>
+        <v>0.119999997</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="E8" s="2">
         <v>21000</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="1"/>
-        <v>3.45544136109991</v>
+        <v>4.3647680350735705</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="B9" s="4">
-        <v>0.47799998500000002</v>
+        <v>0.33000001299999998</v>
       </c>
       <c r="C9" s="4">
-        <v>0.10400000199999999</v>
+        <v>7.8000001999999999E-2</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="E9" s="2">
         <v>21000</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="1"/>
-        <v>2.5461146871262494</v>
+        <v>3.45544136109991</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B10" s="4">
-        <v>0.69199997199999996</v>
+        <v>0.47799998500000002</v>
       </c>
       <c r="C10" s="4">
-        <v>0.14399999399999999</v>
+        <v>0.10400000199999999</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="E10" s="2">
         <v>21000</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="1"/>
-        <v>1.818653347947321</v>
+        <v>2.5461146871262494</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B11" s="4">
-        <v>0.74099999699999997</v>
+        <v>0.69199997199999996</v>
       </c>
       <c r="C11" s="4">
-        <v>0.15999999600000001</v>
+        <v>0.14399999399999999</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="E11" s="2">
         <v>21000</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="1"/>
-        <v>1.2730573435631247</v>
+        <v>1.818653347947321</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12">
+        <v>35</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.74099999699999997</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.15999999600000001</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="E12" s="2">
+        <v>21000</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="1"/>
+        <v>1.2730573435631247</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
         <v>25</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B13" s="4">
         <v>1.2400000099999999</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C13" s="4">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="E12" s="2">
-        <v>21000</v>
-      </c>
-      <c r="F12" s="2">
+      <c r="E13" s="2">
+        <v>21000</v>
+      </c>
+      <c r="F13" s="2">
         <f t="shared" si="1"/>
         <v>0.90932667397366052</v>
       </c>
     </row>
-    <row r="19" spans="7:7">
-      <c r="G19" s="5"/>
+    <row r="20" spans="7:7">
+      <c r="G20" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>